<commit_message>
Inscripcion Registro Automotor terminado
</commit_message>
<xml_diff>
--- a/script_DNRPA/registroInscripcionMotoCorrientes.xlsx
+++ b/script_DNRPA/registroInscripcionMotoCorrientes.xlsx
@@ -480,566 +480,566 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>41640</v>
+        <v>44562</v>
       </c>
       <c r="B2" t="n">
-        <v>294</v>
+        <v>70</v>
       </c>
       <c r="C2" t="n">
-        <v>526</v>
+        <v>247</v>
       </c>
       <c r="D2" t="n">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="E2" t="n">
-        <v>573</v>
+        <v>124</v>
       </c>
       <c r="F2" t="n">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="G2" t="n">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="H2" t="n">
-        <v>165</v>
+        <v>46</v>
       </c>
       <c r="I2" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="J2" t="n">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="K2" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="L2" t="n">
-        <v>529</v>
+        <v>243</v>
       </c>
       <c r="M2" t="n">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="N2" t="n">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="O2" t="n">
-        <v>2760</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>41671</v>
+        <v>44593</v>
       </c>
       <c r="B3" t="n">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="C3" t="n">
-        <v>406</v>
+        <v>317</v>
       </c>
       <c r="D3" t="n">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="E3" t="n">
-        <v>384</v>
+        <v>132</v>
       </c>
       <c r="F3" t="n">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="G3" t="n">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="H3" t="n">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="I3" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="J3" t="n">
+        <v>36</v>
+      </c>
+      <c r="K3" t="n">
+        <v>34</v>
+      </c>
+      <c r="L3" t="n">
+        <v>259</v>
+      </c>
+      <c r="M3" t="n">
+        <v>20</v>
+      </c>
+      <c r="N3" t="n">
         <v>72</v>
       </c>
-      <c r="K3" t="n">
-        <v>64</v>
-      </c>
-      <c r="L3" t="n">
-        <v>358</v>
-      </c>
-      <c r="M3" t="n">
-        <v>39</v>
-      </c>
-      <c r="N3" t="n">
-        <v>73</v>
-      </c>
       <c r="O3" t="n">
-        <v>2002</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>41699</v>
+        <v>44621</v>
       </c>
       <c r="B4" t="n">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="C4" t="n">
-        <v>319</v>
+        <v>378</v>
       </c>
       <c r="D4" t="n">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E4" t="n">
-        <v>327</v>
+        <v>229</v>
       </c>
       <c r="F4" t="n">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G4" t="n">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="H4" t="n">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I4" t="n">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="J4" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="K4" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L4" t="n">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="M4" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="N4" t="n">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="O4" t="n">
-        <v>1768</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>41730</v>
+        <v>44652</v>
       </c>
       <c r="B5" t="n">
-        <v>208</v>
+        <v>110</v>
       </c>
       <c r="C5" t="n">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D5" t="n">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="E5" t="n">
-        <v>374</v>
+        <v>146</v>
       </c>
       <c r="F5" t="n">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="G5" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H5" t="n">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="I5" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J5" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K5" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L5" t="n">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="M5" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="N5" t="n">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="O5" t="n">
-        <v>1683</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>41760</v>
+        <v>44682</v>
       </c>
       <c r="B6" t="n">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="C6" t="n">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="D6" t="n">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="E6" t="n">
-        <v>325</v>
+        <v>195</v>
       </c>
       <c r="F6" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="G6" t="n">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="H6" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I6" t="n">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="J6" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K6" t="n">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="L6" t="n">
-        <v>327</v>
+        <v>270</v>
       </c>
       <c r="M6" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="N6" t="n">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="O6" t="n">
-        <v>1650</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>41791</v>
+        <v>44713</v>
       </c>
       <c r="B7" t="n">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="C7" t="n">
-        <v>307</v>
+        <v>345</v>
       </c>
       <c r="D7" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E7" t="n">
-        <v>232</v>
+        <v>159</v>
       </c>
       <c r="F7" t="n">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="G7" t="n">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="H7" t="n">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="I7" t="n">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J7" t="n">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="K7" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="L7" t="n">
-        <v>268</v>
+        <v>303</v>
       </c>
       <c r="M7" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="N7" t="n">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="O7" t="n">
-        <v>1466</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>41821</v>
+        <v>44743</v>
       </c>
       <c r="B8" t="n">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="C8" t="n">
-        <v>385</v>
+        <v>288</v>
       </c>
       <c r="D8" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E8" t="n">
-        <v>255</v>
+        <v>168</v>
       </c>
       <c r="F8" t="n">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="G8" t="n">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="H8" t="n">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="I8" t="n">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J8" t="n">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="K8" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L8" t="n">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="M8" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="N8" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="O8" t="n">
-        <v>1552</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>41852</v>
+        <v>44774</v>
       </c>
       <c r="B9" t="n">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="C9" t="n">
-        <v>420</v>
+        <v>336</v>
       </c>
       <c r="D9" t="n">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="E9" t="n">
-        <v>257</v>
+        <v>148</v>
       </c>
       <c r="F9" t="n">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G9" t="n">
+        <v>40</v>
+      </c>
+      <c r="H9" t="n">
         <v>65</v>
       </c>
-      <c r="H9" t="n">
-        <v>93</v>
-      </c>
       <c r="I9" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J9" t="n">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="K9" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="L9" t="n">
-        <v>461</v>
+        <v>292</v>
       </c>
       <c r="M9" t="n">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="N9" t="n">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="O9" t="n">
-        <v>1821</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>41883</v>
+        <v>44805</v>
       </c>
       <c r="B10" t="n">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="C10" t="n">
-        <v>379</v>
+        <v>292</v>
       </c>
       <c r="D10" t="n">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="E10" t="n">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="F10" t="n">
+        <v>49</v>
+      </c>
+      <c r="G10" t="n">
+        <v>36</v>
+      </c>
+      <c r="H10" t="n">
         <v>65</v>
       </c>
-      <c r="G10" t="n">
-        <v>94</v>
-      </c>
-      <c r="H10" t="n">
-        <v>126</v>
-      </c>
       <c r="I10" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J10" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K10" t="n">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="L10" t="n">
-        <v>334</v>
+        <v>206</v>
       </c>
       <c r="M10" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="N10" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="O10" t="n">
-        <v>1688</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>41913</v>
+        <v>44835</v>
       </c>
       <c r="B11" t="n">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="C11" t="n">
-        <v>385</v>
+        <v>258</v>
       </c>
       <c r="D11" t="n">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="E11" t="n">
-        <v>257</v>
+        <v>141</v>
       </c>
       <c r="F11" t="n">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="G11" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="H11" t="n">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="I11" t="n">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="J11" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11" t="n">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="L11" t="n">
-        <v>349</v>
+        <v>266</v>
       </c>
       <c r="M11" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="N11" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="O11" t="n">
-        <v>1732</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>41944</v>
+        <v>44866</v>
       </c>
       <c r="B12" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C12" t="n">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="D12" t="n">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="E12" t="n">
-        <v>229</v>
+        <v>135</v>
       </c>
       <c r="F12" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G12" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H12" t="n">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="I12" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J12" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="K12" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="L12" t="n">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="M12" t="n">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="N12" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="O12" t="n">
-        <v>1314</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>41974</v>
+        <v>44896</v>
       </c>
       <c r="B13" t="n">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="C13" t="n">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="D13" t="n">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="E13" t="n">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="F13" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G13" t="n">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="H13" t="n">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="I13" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="J13" t="n">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="K13" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L13" t="n">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="M13" t="n">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="N13" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="O13" t="n">
-        <v>1130</v>
+        <v>745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>